<commit_message>
Update der Aufwände mit geleisteten Stunden
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas Huwe\Documents\Essential Blog\Git\Notizen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Datum</t>
   </si>
@@ -63,6 +63,10 @@
   </si>
   <si>
     <t>Stunden</t>
+  </si>
+  <si>
+    <t>- Einlesen in PHP
+- PHP /MYSQL-Verbindung testen</t>
   </si>
 </sst>
 </file>
@@ -144,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -170,6 +174,9 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -453,7 +460,7 @@
   <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,11 +500,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>41971</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -527,7 +542,7 @@
       </c>
       <c r="G7" s="12">
         <f>SUM(D:D)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Aufwand für HTML eingetragen
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadine\Documents\#GitHub\EssentialBlog\Notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Datum</t>
   </si>
@@ -67,6 +67,9 @@
   <si>
     <t>- Einlesen in PHP
 - PHP /MYSQL-Verbindung testen</t>
+  </si>
+  <si>
+    <t>- 1. Version der HTML-Dokumente (index + Anlegen eines Artikels)</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -177,6 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -460,7 +464,7 @@
   <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,10 +519,18 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="2">
+        <v>41978</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -542,7 +554,7 @@
       </c>
       <c r="G7" s="12">
         <f>SUM(D:D)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
- Bilder gedreht - Aufwände ergenzt - CSS angefangen (Positionierung, Textart) - HTML etwas um Beispieltext (Lorem Ipsum) ergänzt - Style aus dem HTML entfernt - Bitte nicht an den Rahmen stören. Diese sind nur zur Besserung Orientierung beim Programmieren
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadine\Documents\#GitHub\EssentialBlog\Notizen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas Huwe\Documents\Essential Blog\Git\Notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -70,6 +70,10 @@
   </si>
   <si>
     <t>- 1. Version der HTML-Dokumente (index + Anlegen eines Artikels)</t>
+  </si>
+  <si>
+    <t>- Erste Version vom CSS (Anordnung von Kategorien, Überschrift, Filter, Neu, Schriftart, Größe)
+- Habe mit "Lorem Ipsum" den Text des Beispielartikels erweitert</t>
   </si>
 </sst>
 </file>
@@ -464,12 +468,12 @@
   <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.140625" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
@@ -532,11 +536,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>41982</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -554,7 +566,7 @@
       </c>
       <c r="G7" s="12">
         <f>SUM(D:D)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Änderungen: -MYSQL-Datenbank erstellt -MYSQL-Datenbank mit Testdaten gefüllt -HTML-File von Nadine/ Lukas in php-File umgewandelt -Großteil der variablen Begriffe durch php-Funktionen dynamisch aus MYSQL-DB abgefragt -Bilder in Ordner Images verschoben und Pfade in index.php angepasst
Erklärung Dateien:
-index.php wird initial aufgerufen und läd connection.php + function.php
-connection.php baut DB Verbindung auf
-function.php beinhaltet MYSQL-Statements
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas Huwe\Documents\Essential Blog\Git\Notizen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Datum</t>
   </si>
@@ -74,6 +74,15 @@
   <si>
     <t>- Erste Version vom CSS (Anordnung von Kategorien, Überschrift, Filter, Neu, Schriftart, Größe)
 - Habe mit "Lorem Ipsum" den Text des Beispielartikels erweitert</t>
+  </si>
+  <si>
+    <t>- MYSQL-Datenbank erstellt
+- HTML-File von Nadine in PHP umgewandelt (mithilfe von Converter)
+- PHP Funktionen gebaut und in HMTL-Struktur eingebaut</t>
+  </si>
+  <si>
+    <t>- PHP-Funtionen gebaut
+- PHP-Funktionen mit HTML-Dokument von Lukas gemerged</t>
   </si>
 </sst>
 </file>
@@ -155,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -185,6 +194,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -465,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H147"/>
+  <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,227 +548,243 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>41981</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>41982</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D6" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="F7" s="12" t="s">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>41982</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="F8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>9</v>
-      </c>
-      <c r="H7" s="12" t="s">
+        <v>14.5</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -1411,6 +1439,12 @@
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
XAMP installiert, DB eingerichtet und Einarbeitung in Javascript
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Erfassung" sheetId="1" r:id="rId1"/>
     <sheet name="Legende" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -83,16 +78,25 @@
   <si>
     <t>- PHP-Funtionen gebaut
 - PHP-Funktionen mit HTML-Dokument von Lukas gemerged</t>
+  </si>
+  <si>
+    <t>Mittwoch, 10. Dezember 2014</t>
+  </si>
+  <si>
+    <t>- XAMP installiert
+'- Datenbank eingerichtet
+'- Einarbeitung in den aktuellen Entwicklungsstand
+'- Einarbeitung in Javascript</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,7 +261,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,7 +296,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,30 +473,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.140625" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -506,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" s="4">
         <v>41971</v>
       </c>
@@ -520,7 +524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30">
       <c r="A3" s="9">
         <v>41971</v>
       </c>
@@ -534,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>41978</v>
       </c>
@@ -548,7 +552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" s="2">
         <v>41981</v>
       </c>
@@ -562,7 +566,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45">
       <c r="A6" s="9">
         <v>41982</v>
       </c>
@@ -576,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30">
       <c r="A7" s="2">
         <v>41982</v>
       </c>
@@ -590,857 +594,865 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+    <row r="8" spans="1:8" ht="60.75">
+      <c r="A8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2</v>
+      </c>
       <c r="F8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="9"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="9"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="9"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="9"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="2"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="2"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="2"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="2"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="2"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="2"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="2"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" s="2"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="2"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="2"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="2"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" s="2"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" s="2"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" s="2"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" s="2"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" s="2"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" s="2"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" s="2"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" s="2"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" s="2"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" s="2"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" s="2"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" s="2"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" s="2"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" s="2"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" s="2"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" s="2"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" s="2"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" s="2"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -1465,36 +1477,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Aufwände aktualisiert - Zu diesem Entwicklungsstand funktionieren die Javascript Funktionen noch nicht (Wahrscheinlich eine Kleinigkeit) - Vervollständigung der Javascript Funktionen zu einem späteren Termin
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="12435"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="Erfassung" sheetId="1" r:id="rId1"/>
     <sheet name="Legende" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Datum</t>
   </si>
@@ -99,15 +94,24 @@
 - Sortiermöglichkeit umgesetzt (URL-Parameter: &amp;order=) (noch nicht in Dropdown-Menü Sortierung eingebaut)
 - Möglichkeit Anzahl der angezeigten Artikel zu begrenzen (URL-Parameter: &amp;displayedarticles= )</t>
   </si>
+  <si>
+    <t>Donnerstag, 11. Dezember 2014</t>
+  </si>
+  <si>
+    <t>- Manchen Elementen im HTML Ids und Klassen zugeordnet
+'- Javascript Funktionen zum Anzeigen und Verstecken implementiert
+'- Javascript in PHP Datei eingebunden
+'- CSS erweitert, sodass manche Elemente nun initial unsichtbar sind</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,30 +488,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.140625" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -521,7 +525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" s="4">
         <v>41971</v>
       </c>
@@ -535,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30">
       <c r="A3" s="9">
         <v>41971</v>
       </c>
@@ -549,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>41978</v>
       </c>
@@ -563,7 +567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" s="2">
         <v>41981</v>
       </c>
@@ -577,7 +581,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="45">
       <c r="A6" s="9">
         <v>41982</v>
       </c>
@@ -591,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30">
       <c r="A7" s="2">
         <v>41982</v>
       </c>
@@ -605,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="60.75">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -623,13 +627,13 @@
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>18.5</v>
+        <v>21.5</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="105">
       <c r="A9" s="2">
         <v>41983</v>
       </c>
@@ -643,835 +647,843 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="90">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="9"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="9"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="9"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="2"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="2"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="2"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="2"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="2"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="2"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="2"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" s="2"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="2"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="2"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="2"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" s="2"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" s="2"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" s="2"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" s="2"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" s="2"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" s="2"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" s="2"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" s="2"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" s="2"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" s="2"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" s="2"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" s="2"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" s="2"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" s="2"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" s="2"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" s="2"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" s="2"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" s="2"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -1496,36 +1508,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Fehlersuche im Javascript Part - HTML geringfügig verändert - alert() Meldungen zur Fehlersuche ins Javascript eingebaut - Aufwände angepasst
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -102,6 +102,13 @@
 '- Javascript Funktionen zum Anzeigen und Verstecken implementiert
 '- Javascript in PHP Datei eingebunden
 '- CSS erweitert, sodass manche Elemente nun initial unsichtbar sind</t>
+  </si>
+  <si>
+    <t>Mittwoch, 17. Dezember 2014</t>
+  </si>
+  <si>
+    <t>- HTML geringfügig verändert
+- alert() Meldungen ins Javascript eingebaut, um Fehlersuche betreiben zu können</t>
   </si>
 </sst>
 </file>
@@ -488,7 +495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -499,7 +506,7 @@
   <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -627,7 +634,7 @@
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>21.5</v>
+        <v>22</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
@@ -661,11 +668,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+    <row r="11" spans="1:8" ht="45">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="9"/>

</xml_diff>

<commit_message>
Kommentare können nun ausgeklappt und wieder eingeklappt werden - format.css: Kommentare sind initial eingeklappt - clientFunctions.js: Scricptfehler beseitigt; Es werden nun andere Eigenschaften im DOM geändert - Aufwände aktualisiert
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -98,17 +98,25 @@
     <t>Donnerstag, 11. Dezember 2014</t>
   </si>
   <si>
-    <t>- Manchen Elementen im HTML Ids und Klassen zugeordnet
-'- Javascript Funktionen zum Anzeigen und Verstecken implementiert
-'- Javascript in PHP Datei eingebunden
-'- CSS erweitert, sodass manche Elemente nun initial unsichtbar sind</t>
-  </si>
-  <si>
     <t>Mittwoch, 17. Dezember 2014</t>
   </si>
   <si>
     <t>- HTML geringfügig verändert
 - alert() Meldungen ins Javascript eingebaut, um Fehlersuche betreiben zu können</t>
+  </si>
+  <si>
+    <t>Donnerstag, 18. Dezember 2014</t>
+  </si>
+  <si>
+    <t>- Manchen Elementen im HTML Ids und Klassen zugeordnet
+- Javascript Funktionen zum Anzeigen und Verstecken implementiert
+- Javascript in PHP Datei eingebunden
+- CSS erweitert, sodass manche Elemente nun initial unsichtbar sind</t>
+  </si>
+  <si>
+    <t>- Weitere alert() Meldungen ins Javascript eingebaut, um die auftretenden Fehler weiter einzugrenzen
+- CSS erweitert Kommentare werden nun initial nicht angezeigt
+- Javascript korrigiert: Scriptfehler beseitigt; Beim Anzeigen oder Verstecken von Kommentaren werden nun die korrekten Eigenschaften im DOM geändert</t>
   </si>
 </sst>
 </file>
@@ -495,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,7 +514,7 @@
   <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -634,7 +642,7 @@
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>22</v>
+        <v>23.5</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
@@ -662,7 +670,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" s="10">
         <v>3</v>
@@ -670,23 +678,31 @@
     </row>
     <row r="11" spans="1:8" ht="45">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+    <row r="12" spans="1:8" ht="90">
+      <c r="A12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2"/>

</xml_diff>

<commit_message>
Neuer Artikel kann erstellt werden (Kategorie wird aktuell nicht übergeben
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="12435"/>
   </bookViews>
@@ -10,9 +15,9 @@
     <sheet name="Erfassung" sheetId="1" r:id="rId1"/>
     <sheet name="Legende" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Datum</t>
   </si>
@@ -118,15 +123,20 @@
 - CSS erweitert Kommentare werden nun initial nicht angezeigt
 - Javascript korrigiert: Scriptfehler beseitigt; Beim Anzeigen oder Verstecken von Kommentaren werden nun die korrekten Eigenschaften im DOM geändert</t>
   </si>
+  <si>
+    <t>-Sortiermöglichkeit umgesetzt
+ -Artikel erstellen bis auf Kategorieübergabe umgesetzt
+ -JavaScript Datei verschoben in include-Ordner</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,21 +513,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -526,7 +536,7 @@
     <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -540,7 +550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>41971</v>
       </c>
@@ -554,7 +564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>41971</v>
       </c>
@@ -568,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>41978</v>
       </c>
@@ -582,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41981</v>
       </c>
@@ -596,7 +606,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>41982</v>
       </c>
@@ -610,7 +620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>41982</v>
       </c>
@@ -624,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60.75">
+    <row r="8" spans="1:8" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -642,13 +652,13 @@
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>23.5</v>
+        <v>26.5</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="105">
+    <row r="9" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>41983</v>
       </c>
@@ -662,7 +672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="90">
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
@@ -676,7 +686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -690,7 +700,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="90">
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
@@ -704,817 +714,825 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:8">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>42020</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -1539,36 +1557,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Abstimmung in Aufwands-Excel eingetragen
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadine\Documents\#GitHub\EssentialBlog\Notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Datum</t>
   </si>
@@ -127,6 +127,20 @@
     <t>-Sortiermöglichkeit umgesetzt
  -Artikel erstellen bis auf Kategorieübergabe umgesetzt
  -JavaScript Datei verschoben in include-Ordner</t>
+  </si>
+  <si>
+    <t>alle</t>
+  </si>
+  <si>
+    <t>Besprechung: noch zu implementieren:
+- Like-Funktion (S)
+- Kommentar-Funktion (S)
+- Kategorie an einem Artikel speichern (S)
+- Design verschönern (L)
+         - Kästen oben weg
+         - Arial
+         - Hintergrund: Farbverlauf
+- vernünftige Testdaten (Artikel + Kommentare) in DB einfügen (N)</t>
   </si>
 </sst>
 </file>
@@ -208,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -239,6 +253,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -652,7 +669,7 @@
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>26.5</v>
+        <v>26.75</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
@@ -728,11 +745,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+    <row r="14" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>42021</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>

</xml_diff>

<commit_message>
- Kommentar-Funktion - Artikel-Like-Funktion - Kommentar-Like-Funktion - Querverweise - Kleinigkeiten
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadine\Documents\#GitHub\EssentialBlog\Notizen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Datum</t>
   </si>
@@ -141,6 +141,13 @@
          - Arial
          - Hintergrund: Farbverlauf
 - vernünftige Testdaten (Artikel + Kommentare) in DB einfügen (N)</t>
+  </si>
+  <si>
+    <t>- Kommentar-Funktion
+- Artikel-Like-Funktion
+- Kommentar-Like-Funktion
+- Querverweise
+- Kleinigkeiten</t>
   </si>
 </sst>
 </file>
@@ -541,7 +548,7 @@
   <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +676,7 @@
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>26.75</v>
+        <v>29.75</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
@@ -759,11 +766,19 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>42023</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>

</xml_diff>

<commit_message>
Aufwand für Demodaten nachgetragen
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadine\Documents\#GitHub\EssentialBlog\Notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Datum</t>
   </si>
@@ -148,6 +148,12 @@
 - Kommentar-Like-Funktion
 - Querverweise
 - Kleinigkeiten</t>
+  </si>
+  <si>
+    <t>17. + 19.01.2015</t>
+  </si>
+  <si>
+    <t>Skript zum Einfügen sinnvollerer Demodaten erstellt</t>
   </si>
 </sst>
 </file>
@@ -229,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -264,6 +270,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +685,7 @@
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>29.75</v>
+        <v>33.75</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
@@ -781,10 +790,18 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>

</xml_diff>

<commit_message>
- Nadines Daten als MYSQL-Dump umgebaut um FK-Probleme zu vermeiden - Umlaute in Nadines Daten ausgebessert, da sonst Darstellungsfehler entstanden sind - Sortierfunktion zeigt aktuelle Selektion aus - falls aktiver Kategoriefilter gesetzt ist, wird die entsprechende Kategorie gehighlighted - beim Erstellen eines neuen Artikels kann eine bestehende Kategorie ausgewählt werden - es können neue Kategorien erstellt werden - es erfolgen Prüfungen, ob alle Felder bei Speicherung von Kategorie/Artikel/Kommentar gespeichert sind - Anzeige des Erstellungsdatums aufgehüptscht
</commit_message>
<xml_diff>
--- a/Notizen/Aufwände.xlsx
+++ b/Notizen/Aufwände.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadine\Documents\#GitHub\EssentialBlog\Notizen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soch\Documents\GitHub\EssentialBlog\Notizen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Datum</t>
   </si>
@@ -154,6 +154,17 @@
   </si>
   <si>
     <t>Skript zum Einfügen sinnvollerer Demodaten erstellt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Nadines Daten als MYSQL-Dump umgebaut um FK-Probleme zu vermeiden
+- Umlaute in Nadines Daten ausgebessert, da sonst Darstellungsfehler entstanden sind
+- Sortierfunktion zeigt aktuelle Selektion aus
+- falls aktiver Kategoriefilter gesetzt ist, wird die entsprechende Kategorie gehighlighted
+- beim Erstellen eines neuen Artikels kann eine bestehende Kategorie ausgewählt werden
+- es können neue Kategorien erstellt werden
+- es erfolgen Prüfungen, ob alle Felder bei Speicherung von Kategorie/Artikel/Kommentar gespeichert sind
+- Anzeige des Erstellungsdatums aufgehüptscht
+</t>
   </si>
 </sst>
 </file>
@@ -556,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +696,7 @@
       </c>
       <c r="G8" s="12">
         <f>SUM(D:D)</f>
-        <v>33.75</v>
+        <v>37.75</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>11</v>
@@ -803,11 +814,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+    <row r="17" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>42024</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>

</xml_diff>